<commit_message>
authform and configform style update
</commit_message>
<xml_diff>
--- a/machines.xlsx
+++ b/machines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="313">
   <si>
     <t>MCD CODE</t>
   </si>
@@ -960,6 +960,9 @@
   </si>
   <si>
     <t>Most updated mcd with SPIFFS</t>
+  </si>
+  <si>
+    <t>Trouble</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1021,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1061,6 +1064,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1083,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1091,9 +1100,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1141,6 +1147,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1153,7 +1163,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1232,11 +1249,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="306364144"/>
-        <c:axId val="306365712"/>
+        <c:axId val="366085736"/>
+        <c:axId val="366085344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="306364144"/>
+        <c:axId val="366085736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306365712"/>
+        <c:crossAx val="366085344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1286,7 +1303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="306365712"/>
+        <c:axId val="366085344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1353,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306364144"/>
+        <c:crossAx val="366085736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1441,11 +1458,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="306363360"/>
-        <c:axId val="306366104"/>
+        <c:axId val="367167736"/>
+        <c:axId val="367167344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="306363360"/>
+        <c:axId val="367167736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306366104"/>
+        <c:crossAx val="367167344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1495,7 +1512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="306366104"/>
+        <c:axId val="367167344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,7 +1562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306363360"/>
+        <c:crossAx val="367167736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3040,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,7 +3066,7 @@
     <col min="1" max="1" width="17.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="54.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="2" customWidth="1"/>
@@ -3083,959 +3100,962 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
     </row>
     <row r="2" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
     <row r="3" spans="1:33" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="G3" s="32" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="G3" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="N3" s="33" t="s">
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="N3" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
       <c r="W3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="6" t="s">
         <v>213</v>
       </c>
       <c r="W4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="31">
         <v>10007</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="19">
         <v>1000395</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="14">
         <v>1000416</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="S5" s="13" t="s">
         <v>195</v>
       </c>
       <c r="W5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>100061</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="39">
         <v>100010</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="14">
         <v>1000298</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="13" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="31">
         <v>10002</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <v>1000269</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="21"/>
-      <c r="N7" s="14" t="s">
+      <c r="L7" s="20"/>
+      <c r="N7" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="14">
         <v>1000256</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="R7" s="14" t="s">
+      <c r="R7" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="S7" s="14" t="s">
+      <c r="S7" s="13" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>1000292</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="39">
         <v>1000392</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="14" t="s">
+      <c r="M8" s="8"/>
+      <c r="N8" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="14">
         <v>100072</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="Q8" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="R8" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="S8" s="13" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="31">
         <v>1000148</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="39">
         <v>100076</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="14" t="s">
+      <c r="M9" s="8"/>
+      <c r="N9" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="14">
         <v>1000240</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="P9" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="Q9" s="17" t="s">
+      <c r="Q9" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R9" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="S9" s="14" t="s">
+      <c r="S9" s="13" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="31">
         <v>1000265</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="21">
         <v>100015</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="13"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="31">
         <v>100035</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="29">
         <v>1000170</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="29" t="s">
+      <c r="L11" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="13"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="31">
         <v>1000180</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="19">
         <v>100060</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="13"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="31">
         <v>1000437</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="19">
         <v>1000173</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="L13" s="19" t="s">
+      <c r="L13" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="13"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>100014</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="19">
         <v>100017</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="13"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>10008</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="19">
         <v>100068</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="13"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="31">
         <v>100038</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="19">
         <v>100071</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="13"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="37">
         <v>1000299</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="19">
         <v>100019</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="13"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>1000207</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="19">
         <v>100082</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L18" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="13"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="39">
         <v>1000304</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="L19" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="13"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="21">
         <v>1000241</v>
       </c>
-      <c r="I20" s="21" t="s">
+      <c r="I20" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="K20" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="L20" s="21"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="13"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="19">
         <v>100020</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="L21" s="19" t="s">
+      <c r="L21" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="13"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="12"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
       <c r="C22" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="19">
         <v>100096</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="L22" s="19" t="s">
+      <c r="L22" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="13"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="12"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="13"/>
       <c r="C23" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="19">
         <v>100070</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="19" t="s">
+      <c r="L23" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="13"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="12"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="G24" s="19" t="s">
+      <c r="A24" s="4"/>
+      <c r="C24" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G24" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="19">
         <v>100016</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="13"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="12"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="G25" s="19" t="s">
+      <c r="A25" s="8"/>
+      <c r="G25" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="19">
         <v>100074</v>
       </c>
-      <c r="I25" s="23" t="s">
+      <c r="I25" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="L25" s="19" t="s">
+      <c r="L25" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="13"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="12"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="30"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
+      <c r="A27" s="8"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="8"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4067,296 +4087,296 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>200031</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>200061</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>200028</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>20005</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>200074</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>2000106</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>20006</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>200080</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>200098</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>200081</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>200032</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>200055</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>200033</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>200035</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>200097</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="13"/>
       <c r="C22" s="2" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="5"/>
       <c r="C23" s="2" t="s">
         <v>190</v>
       </c>
@@ -4395,295 +4415,295 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="2" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>300024</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>3000110</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>300094</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>3000127</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>3000124</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>300032</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>300028</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>3000132</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>3000113</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>300097</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>3000109</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>300052</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>3000126</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>300040</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>3000107</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>307</v>
       </c>
     </row>
@@ -4724,36 +4744,36 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>180</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -4761,22 +4781,22 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>800022</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -4784,22 +4804,22 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>800041</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -4807,22 +4827,22 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>800013</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -4830,22 +4850,22 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>800023</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -4853,22 +4873,22 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>800011</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -4876,22 +4896,22 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>800040</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -4899,22 +4919,22 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>800017</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -4922,22 +4942,22 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>800012</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -4945,22 +4965,22 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="25">
         <v>800039</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="24" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -4968,22 +4988,22 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>80008</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -4991,22 +5011,22 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>800014</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -5014,22 +5034,22 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>800037</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -5037,22 +5057,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>800026</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -5060,22 +5080,22 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <v>800016</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -5083,22 +5103,22 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="14">
         <v>800024</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -5106,22 +5126,22 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <v>800015</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -5129,22 +5149,22 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="14">
         <v>800049</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -5152,22 +5172,22 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="14">
         <v>800020</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -5175,22 +5195,22 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="14">
         <v>80007</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -5198,22 +5218,22 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="14">
         <v>80005</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -5221,22 +5241,22 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="14">
         <v>800038</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G26" s="2" t="s">

</xml_diff>

<commit_message>
added router tab in machines.xlxs
</commit_message>
<xml_diff>
--- a/machines.xlsx
+++ b/machines.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19095" windowHeight="7425" tabRatio="308" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19095" windowHeight="7425" tabRatio="308" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Chart2" sheetId="9" r:id="rId1"/>
     <sheet name="Chart1" sheetId="8" r:id="rId2"/>
     <sheet name="North" sheetId="1" r:id="rId3"/>
-    <sheet name="Central" sheetId="7" r:id="rId4"/>
-    <sheet name="South" sheetId="4" r:id="rId5"/>
-    <sheet name="Bohol" sheetId="6" r:id="rId6"/>
+    <sheet name="Routers" sheetId="10" r:id="rId4"/>
+    <sheet name="Central" sheetId="7" r:id="rId5"/>
+    <sheet name="South" sheetId="4" r:id="rId6"/>
+    <sheet name="Bohol" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="371">
   <si>
     <t>MCD CODE</t>
   </si>
@@ -999,13 +1000,151 @@
   </si>
   <si>
     <t>192.168.1.96</t>
+  </si>
+  <si>
+    <t>Hobart</t>
+  </si>
+  <si>
+    <t>192.168.1.97</t>
+  </si>
+  <si>
+    <t>BA(200)-Grinding - (207) Conrod Assy</t>
+  </si>
+  <si>
+    <t>200-207-102-Y210-100MM-SNN</t>
+  </si>
+  <si>
+    <t>SSID</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>LAN IP</t>
+  </si>
+  <si>
+    <t>SUBNET MASK</t>
+  </si>
+  <si>
+    <t>WAN IP</t>
+  </si>
+  <si>
+    <t>DEFAULT GATEWAY</t>
+  </si>
+  <si>
+    <t>DNS SERVER 1</t>
+  </si>
+  <si>
+    <t>Wifi_South</t>
+  </si>
+  <si>
+    <t>(---WifiSouth---)</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>WmdcPassword5432</t>
+  </si>
+  <si>
+    <t>192.168.2.90</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>192.168.2.101</t>
+  </si>
+  <si>
+    <t>Wifi_Central</t>
+  </si>
+  <si>
+    <t>(---WifiCentral---)</t>
+  </si>
+  <si>
+    <t>192.168.3.29</t>
+  </si>
+  <si>
+    <t>192.168.1.89</t>
+  </si>
+  <si>
+    <t>192.168.1.52</t>
+  </si>
+  <si>
+    <t>Wifi_Er</t>
+  </si>
+  <si>
+    <t>192.168.1.100</t>
+  </si>
+  <si>
+    <t>wifi_mf2</t>
+  </si>
+  <si>
+    <t>192.168.2.100</t>
+  </si>
+  <si>
+    <t>Wifi_Mf</t>
+  </si>
+  <si>
+    <t>wmdcwifimf</t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Bohol</t>
+  </si>
+  <si>
+    <t>Access Point</t>
+  </si>
+  <si>
+    <t>North ER</t>
+  </si>
+  <si>
+    <t>North MF Finance</t>
+  </si>
+  <si>
+    <t>192.168.1.3</t>
+  </si>
+  <si>
+    <t>255.255.255.1</t>
+  </si>
+  <si>
+    <t>wmdcwifier</t>
+  </si>
+  <si>
+    <t>wmdc_1959</t>
+  </si>
+  <si>
+    <t>Forgotten</t>
+  </si>
+  <si>
+    <t>North MF&amp;DHI Main</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1055,6 +1194,19 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1107,7 +1259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1124,11 +1276,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1175,10 +1357,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1209,6 +1387,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1288,11 +1475,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="361407328"/>
-        <c:axId val="361403800"/>
+        <c:axId val="353877576"/>
+        <c:axId val="353880712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361407328"/>
+        <c:axId val="353877576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +1521,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361403800"/>
+        <c:crossAx val="353880712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1342,7 +1529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361403800"/>
+        <c:axId val="353880712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,7 +1579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361407328"/>
+        <c:crossAx val="353877576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1497,11 +1684,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="361407720"/>
-        <c:axId val="361408112"/>
+        <c:axId val="353873264"/>
+        <c:axId val="353877184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361407720"/>
+        <c:axId val="353873264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,7 +1730,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361408112"/>
+        <c:crossAx val="353877184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1551,7 +1738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361408112"/>
+        <c:axId val="353877184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361407720"/>
+        <c:crossAx val="353873264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3096,15 +3283,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29:K30"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38" style="2" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="2" customWidth="1"/>
@@ -3170,29 +3357,29 @@
       <c r="AG2" s="3"/>
     </row>
     <row r="3" spans="1:36" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="36"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="Q3" s="39" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="34"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="Q3" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
       <c r="Z3" s="3"/>
       <c r="AG3" s="3"/>
     </row>
@@ -3261,28 +3448,28 @@
       <c r="AG4" s="3"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="31">
         <v>10007</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H5" s="32"/>
+      <c r="H5" s="30"/>
       <c r="J5" s="18" t="s">
         <v>11</v>
       </c>
@@ -3323,46 +3510,46 @@
       <c r="AG5" s="3"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="31">
         <v>100061</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="33">
         <v>100010</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="M6" s="34" t="s">
+      <c r="M6" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="N6" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="O6" s="32" t="s">
         <v>198</v>
       </c>
       <c r="Q6" s="13" t="s">
@@ -3385,28 +3572,28 @@
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="31">
         <v>10002</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="30" t="s">
         <v>318</v>
       </c>
       <c r="I7" s="8"/>
@@ -3446,46 +3633,46 @@
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="31">
         <v>1000292</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="33">
         <v>1000392</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="M8" s="34" t="s">
+      <c r="M8" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="34" t="s">
+      <c r="N8" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="32" t="s">
         <v>198</v>
       </c>
       <c r="P8" s="8"/>
@@ -3509,46 +3696,46 @@
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="31">
         <v>1000148</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="29">
         <v>100076</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="N9" s="30" t="s">
+      <c r="N9" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="O9" s="28" t="s">
         <v>198</v>
       </c>
       <c r="P9" s="8"/>
@@ -3572,28 +3759,28 @@
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="31">
         <v>1000265</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="30" t="s">
         <v>318</v>
       </c>
       <c r="J10" s="20" t="s">
@@ -3621,46 +3808,46 @@
       <c r="T10" s="12"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="31">
         <v>100035</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="27">
         <v>1000170</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="N11" s="28" t="s">
+      <c r="N11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="28" t="s">
+      <c r="O11" s="26" t="s">
         <v>193</v>
       </c>
       <c r="P11" s="8"/>
@@ -3670,46 +3857,46 @@
       <c r="T11" s="12"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="31">
         <v>1000180</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="35">
+      <c r="K12" s="33">
         <v>100060</v>
       </c>
-      <c r="L12" s="34" t="s">
+      <c r="L12" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="M12" s="34" t="s">
+      <c r="M12" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="N12" s="34" t="s">
+      <c r="N12" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="32" t="s">
         <v>193</v>
       </c>
       <c r="P12" s="8"/>
@@ -3719,46 +3906,46 @@
       <c r="T12" s="12"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="31">
         <v>1000437</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="30" t="s">
         <v>237</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="35">
+      <c r="K13" s="33">
         <v>1000173</v>
       </c>
-      <c r="L13" s="34" t="s">
+      <c r="L13" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="M13" s="34" t="s">
+      <c r="M13" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="N13" s="34" t="s">
+      <c r="N13" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="O13" s="34" t="s">
+      <c r="O13" s="32" t="s">
         <v>198</v>
       </c>
       <c r="P13" s="8"/>
@@ -3768,46 +3955,46 @@
       <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="31">
         <v>100014</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="33">
         <v>100017</v>
       </c>
-      <c r="L14" s="34" t="s">
+      <c r="L14" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="M14" s="34" t="s">
+      <c r="M14" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="N14" s="34" t="s">
+      <c r="N14" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="34" t="s">
+      <c r="O14" s="32" t="s">
         <v>193</v>
       </c>
       <c r="P14" s="8"/>
@@ -3817,28 +4004,28 @@
       <c r="T14" s="12"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="31">
         <v>10008</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="30"/>
       <c r="J15" s="18" t="s">
         <v>33</v>
       </c>
@@ -3864,46 +4051,46 @@
       <c r="T15" s="12"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="31">
         <v>100038</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="35">
+      <c r="K16" s="33">
         <v>100071</v>
       </c>
-      <c r="L16" s="34" t="s">
+      <c r="L16" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="M16" s="34" t="s">
+      <c r="M16" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="N16" s="34" t="s">
+      <c r="N16" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="O16" s="34" t="s">
+      <c r="O16" s="32" t="s">
         <v>198</v>
       </c>
       <c r="P16" s="8"/>
@@ -3913,46 +4100,46 @@
       <c r="T16" s="12"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="31">
         <v>1000299</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J17" s="34" t="s">
+      <c r="J17" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="33">
         <v>100019</v>
       </c>
-      <c r="L17" s="34" t="s">
+      <c r="L17" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="M17" s="34" t="s">
+      <c r="M17" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="N17" s="34" t="s">
+      <c r="N17" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="O17" s="34" t="s">
+      <c r="O17" s="32" t="s">
         <v>198</v>
       </c>
       <c r="P17" s="8"/>
@@ -3962,46 +4149,46 @@
       <c r="T17" s="12"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="31">
         <v>1000207</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="J18" s="34" t="s">
+      <c r="J18" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="33">
         <v>100082</v>
       </c>
-      <c r="L18" s="34" t="s">
+      <c r="L18" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="M18" s="34" t="s">
+      <c r="M18" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="O18" s="34" t="s">
+      <c r="O18" s="32" t="s">
         <v>193</v>
       </c>
       <c r="P18" s="8"/>
@@ -4011,44 +4198,44 @@
       <c r="T18" s="12"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="30" t="s">
         <v>279</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="31">
         <v>1000414</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="J19" s="34" t="s">
+      <c r="H19" s="30"/>
+      <c r="J19" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="33">
         <v>1000304</v>
       </c>
-      <c r="L19" s="34" t="s">
+      <c r="L19" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="M19" s="34" t="s">
+      <c r="M19" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="N19" s="34" t="s">
+      <c r="N19" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="O19" s="34" t="s">
+      <c r="O19" s="32" t="s">
         <v>193</v>
       </c>
       <c r="P19" s="8"/>
@@ -4058,22 +4245,44 @@
       <c r="T19" s="12"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J20" s="34" t="s">
+      <c r="A20" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="B20" s="31">
+        <v>1000157</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="J20" s="32" t="s">
         <v>319</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="33">
         <v>1000241</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="M20" s="34" t="s">
+      <c r="M20" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="N20" s="34" t="s">
+      <c r="N20" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="32" t="s">
         <v>198</v>
       </c>
       <c r="P20" s="8"/>
@@ -4083,22 +4292,22 @@
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J21" s="34" t="s">
+      <c r="J21" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="K21" s="35">
+      <c r="K21" s="33">
         <v>100020</v>
       </c>
-      <c r="L21" s="34" t="s">
+      <c r="L21" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="M21" s="34" t="s">
+      <c r="M21" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="N21" s="34" t="s">
+      <c r="N21" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="O21" s="34" t="s">
+      <c r="O21" s="32" t="s">
         <v>198</v>
       </c>
       <c r="P21" s="8"/>
@@ -4108,22 +4317,22 @@
       <c r="T21" s="12"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="33">
         <v>100096</v>
       </c>
-      <c r="L22" s="34" t="s">
+      <c r="L22" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="M22" s="34" t="s">
+      <c r="M22" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="N22" s="34" t="s">
+      <c r="N22" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="O22" s="34" t="s">
+      <c r="O22" s="32" t="s">
         <v>193</v>
       </c>
       <c r="P22" s="8"/>
@@ -4183,7 +4392,7 @@
       <c r="T24" s="12"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="30"/>
       <c r="C25" s="2" t="s">
         <v>308</v>
       </c>
@@ -4216,22 +4425,22 @@
       <c r="C26" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="J26" s="32" t="s">
+      <c r="J26" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="K26" s="33">
+      <c r="K26" s="31">
         <v>1000287</v>
       </c>
-      <c r="L26" s="32" t="s">
+      <c r="L26" s="30" t="s">
         <v>322</v>
       </c>
-      <c r="M26" s="32" t="s">
+      <c r="M26" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="N26" s="32" t="s">
+      <c r="N26" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="O26" s="32" t="s">
+      <c r="O26" s="30" t="s">
         <v>198</v>
       </c>
     </row>
@@ -4240,12 +4449,20 @@
       <c r="C27" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="J27" s="26"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
+      <c r="J27" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="K27" s="33">
+        <v>1000141</v>
+      </c>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="O27" s="32" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
@@ -4284,6 +4501,301 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="41" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>330</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>333</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>334</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>335</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>334</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>336</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>360</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>347</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>349</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
+        <v>363</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>351</v>
+      </c>
+      <c r="K4" s="39" t="s">
+        <v>351</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>352</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="J5" s="39" t="s">
+        <v>351</v>
+      </c>
+      <c r="K5" s="39" t="s">
+        <v>351</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="39" t="s">
+        <v>361</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>367</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39" t="s">
+        <v>370</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>354</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>355</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>369</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>369</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>365</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>366</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>351</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>351</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F23"/>
   <sheetViews>
@@ -4302,13 +4814,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -4604,7 +5116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -4642,13 +5154,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -4930,7 +5442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>

</xml_diff>